<commit_message>
Added a couple more coursworks
</commit_message>
<xml_diff>
--- a/MDFDatabase/MDFDatabase/models/Assessments.xlsx
+++ b/MDFDatabase/MDFDatabase/models/Assessments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hwb14182\Documents\MDFDatabase\MDFDatabase\MDFDatabase\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646BAFE1-93E8-4943-9E30-25AE2098A3CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45414165-990B-4C86-958C-ED88242A1634}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" xr2:uid="{616F1B7E-57DC-492A-B3EB-2B51EDB81EBB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="27">
   <si>
     <t>Module</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Online Assessment 1</t>
+  </si>
+  <si>
+    <t>EE270</t>
   </si>
 </sst>
 </file>
@@ -457,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6B0A174-B3E4-47E9-B6C7-92486F387F3A}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,6 +869,9 @@
       <c r="F19" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="G19" s="1">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -888,6 +894,26 @@
       </c>
       <c r="G20" s="1">
         <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="1">
+        <v>60</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>